<commit_message>
History & reports integrated
</commit_message>
<xml_diff>
--- a/cleaned_animal_disease_prediction.xlsx
+++ b/cleaned_animal_disease_prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abbey\Documents\finalyear_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F278F5-A7C8-45BE-B690-433C02F7E14E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1DB963-296A-407F-BEE4-224EBE1A806E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2086,8 +2086,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:X433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="X433" sqref="X433"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B268" sqref="B268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9598,7 +9598,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>183</v>
       </c>
@@ -10169,7 +10169,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="115" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>183</v>
       </c>
@@ -10725,7 +10725,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>183</v>
       </c>
@@ -11219,7 +11219,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>183</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>183</v>
       </c>
@@ -12355,7 +12355,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>183</v>
       </c>
@@ -12917,7 +12917,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>183</v>
       </c>
@@ -13272,7 +13272,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>183</v>
       </c>
@@ -13837,7 +13837,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>183</v>
       </c>
@@ -14399,7 +14399,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="175" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>183</v>
       </c>
@@ -14958,7 +14958,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="183" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -15310,7 +15310,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="188" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="196" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>183</v>
       </c>
@@ -16437,7 +16437,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="204" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>183</v>
       </c>
@@ -17283,7 +17283,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="216" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>183</v>
       </c>
@@ -17848,7 +17848,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="224" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>183</v>
       </c>
@@ -18413,7 +18413,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="232" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>183</v>
       </c>
@@ -19259,7 +19259,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="244" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>183</v>
       </c>
@@ -19818,7 +19818,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="252" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>183</v>
       </c>
@@ -20383,7 +20383,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="260" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>183</v>
       </c>
@@ -20939,7 +20939,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="268" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>183</v>
       </c>
@@ -21507,7 +21507,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="276" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>183</v>
       </c>
@@ -22066,7 +22066,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="284" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>183</v>
       </c>
@@ -22847,7 +22847,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="295" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>183</v>
       </c>
@@ -23412,7 +23412,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="303" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>183</v>
       </c>
@@ -23983,7 +23983,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="311" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>183</v>
       </c>
@@ -24832,7 +24832,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="323" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>183</v>
       </c>
@@ -25394,7 +25394,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="331" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>183</v>
       </c>
@@ -25962,7 +25962,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="339" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>183</v>
       </c>
@@ -26462,7 +26462,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="346" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>183</v>
       </c>
@@ -27033,7 +27033,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="354" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>183</v>
       </c>
@@ -27595,7 +27595,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="362" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>183</v>
       </c>
@@ -28509,7 +28509,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="375" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>183</v>
       </c>
@@ -29077,7 +29077,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="383" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>183</v>
       </c>
@@ -32690,11 +32690,6 @@
         <filter val="Rabbit"/>
       </filters>
     </filterColumn>
-    <filterColumn colId="21">
-      <filters>
-        <filter val="Mange"/>
-      </filters>
-    </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More description added to treatment2
</commit_message>
<xml_diff>
--- a/cleaned_animal_disease_prediction.xlsx
+++ b/cleaned_animal_disease_prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abbey\Documents\finalyear_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30141ADF-7141-41E2-85EE-5AEDC7B0145D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2CD708-33AB-4CD6-A452-CB47881CD66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8812" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8883" uniqueCount="492">
   <si>
     <t>species</t>
   </si>
@@ -1213,9 +1213,6 @@
     <t>Learn more</t>
   </si>
   <si>
-    <t>Swine flu, or H1N1 influenza, is a respiratory disease of pigs caused by type A influenza viruses</t>
-  </si>
-  <si>
     <t>Swine flu, is a respiratory disease of pigs caused by type A influenza viruses</t>
   </si>
   <si>
@@ -1436,6 +1433,72 @@
   </si>
   <si>
     <t>Vaccination, antibiotics for secondary infections, improve husbandry.</t>
+  </si>
+  <si>
+    <t>Conjunctivitis is the inflammation of the conjunctiva (the thin membrane covering the eye and inner eyelids).</t>
+  </si>
+  <si>
+    <t>Feline asthma is a chronic inflammatory airway disease in cats, similar to human asthma. It involves bronchoconstriction (narrowing of the airways) and excessive mucus production, leading to breathing difficulties.</t>
+  </si>
+  <si>
+    <t>Feline calicivirus is a highly contagious respiratory infection in cats, caused by a virus of the Caliciviridae family.</t>
+  </si>
+  <si>
+    <t>Feline chlamydia is a bacterial infection caused by Chlamydia felis. It primarily affects the eyes and upper respiratory tract in cats.</t>
+  </si>
+  <si>
+    <t>Feline coronavirus is a common viral infection in cats, primarily affecting the intestinal tract.</t>
+  </si>
+  <si>
+    <t>Feline herpesvirus, also called feline viral rhinotracheitis (FVR), is a highly contagious and lifelong viral infection caused by Feline Alphaherpesvirus 1. It primarily targets the respiratory tract, eyes, and nasal passages, often leading to chronic or recurrent symptoms.</t>
+  </si>
+  <si>
+    <t>FIV is a lentivirus (similar to HIV in humans) that weakens a cat's immune system over time, making them susceptible to secondary infections. It is not zoonotic (cannot spread to humans).</t>
+  </si>
+  <si>
+    <t>FIP is a fatal, immune-mediated disease caused by a mutation of the feline coronavirus (FCoV). </t>
+  </si>
+  <si>
+    <t>FeLV is a retrovirus that weakens a cat's immune system, making them susceptible to infections, anemia, and cancer (e.g., lymphoma). It is one of the most common and serious infectious diseases in cats.</t>
+  </si>
+  <si>
+    <t>Feline panleukopenia, also known as feline distemper, is a highly contagious and often fatal viral disease caused by the Feline Parvovirus.</t>
+  </si>
+  <si>
+    <t>Feline renal disease, commonly referred to as chronic kidney disease (CKD), is a progressive condition where the kidneys lose their ability to filter waste from the blood effectively.</t>
+  </si>
+  <si>
+    <t>FRDC is a common, highly contagious syndrome affecting the upper respiratory tract of cats, caused by multiple pathogens.</t>
+  </si>
+  <si>
+    <t>Feline respiratory infections are common, highly contagious illnesses affecting a cat's nose, throat, and sinuses.</t>
+  </si>
+  <si>
+    <t>Feline URI is a common, contagious illness affecting the nose, throat, and sinuses of cats.</t>
+  </si>
+  <si>
+    <t>Feline Viral Rhinotracheitis is a highly contagious upper respiratory infection caused by Feline Herpesvirus-1 (FHV-1).</t>
+  </si>
+  <si>
+    <t>Fungal infections in cats are caused by pathogenic fungi that invade the skin, respiratory system, or internal organs. </t>
+  </si>
+  <si>
+    <t>Gastroenteritis refers to inflammation of the stomach and intestines, leading to digestive upset.</t>
+  </si>
+  <si>
+    <t>Hyperthyroidism is a common endocrine disorder in older cats (typically 10+ years) caused by overactive thyroid glands, leading to excessive production of thyroid hormones (T3/T4).</t>
+  </si>
+  <si>
+    <t>Inflammatory Bowel Disease (IBD) is a chronic gastrointestinal disorder characterized by persistent inflammation of the intestinal lining, leading to impaired nutrient absorption and digestive dysfunction.</t>
+  </si>
+  <si>
+    <t>Intestinal parasites are internal worms or protozoa that infect a cat’s digestive tract, leading to malnutrition, diarrhea, and other health issues.</t>
+  </si>
+  <si>
+    <t>Pancreatitis is the inflammation of the pancreas, an organ responsible for producing digestive enzymes and insulin.</t>
+  </si>
+  <si>
+    <t>Ringworm (dermatophytosis) is a fungal infection of the skin, hair, or claws—not caused by a worm.</t>
   </si>
 </sst>
 </file>
@@ -2286,14 +2349,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X433"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AD13" sqref="AD13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="22" max="22" width="55.85546875" customWidth="1"/>
-    <col min="23" max="23" width="70.85546875" customWidth="1"/>
+    <col min="23" max="23" width="143.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -2514,6 +2577,9 @@
       <c r="W3" t="s">
         <v>336</v>
       </c>
+      <c r="X3" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2730,6 +2796,9 @@
       <c r="W6" t="s">
         <v>349</v>
       </c>
+      <c r="X6" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2944,7 +3013,10 @@
         <v>68</v>
       </c>
       <c r="W9" t="s">
-        <v>401</v>
+        <v>400</v>
+      </c>
+      <c r="X9" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -3162,6 +3234,9 @@
       <c r="W12" t="s">
         <v>318</v>
       </c>
+      <c r="X12" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -3307,6 +3382,9 @@
       <c r="W14" t="s">
         <v>318</v>
       </c>
+      <c r="X14" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -3594,6 +3672,9 @@
       <c r="W18" t="s">
         <v>333</v>
       </c>
+      <c r="X18" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -3810,6 +3891,9 @@
       <c r="W21" t="s">
         <v>336</v>
       </c>
+      <c r="X21" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -4097,6 +4181,9 @@
       <c r="W25" t="s">
         <v>318</v>
       </c>
+      <c r="X25" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -4237,7 +4324,7 @@
         <v>104</v>
       </c>
       <c r="W27" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="X27" t="s">
         <v>352</v>
@@ -4311,7 +4398,10 @@
         <v>106</v>
       </c>
       <c r="W28" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X28" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -4382,7 +4472,7 @@
         <v>108</v>
       </c>
       <c r="W29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -4527,7 +4617,10 @@
         <v>110</v>
       </c>
       <c r="W31" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X31" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -4743,7 +4836,10 @@
         <v>111</v>
       </c>
       <c r="W34" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X34" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
@@ -4814,7 +4910,7 @@
         <v>112</v>
       </c>
       <c r="W35" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -4885,7 +4981,7 @@
         <v>113</v>
       </c>
       <c r="W36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -5032,6 +5128,9 @@
       <c r="W38" t="s">
         <v>344</v>
       </c>
+      <c r="X38" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
@@ -5101,7 +5200,7 @@
         <v>116</v>
       </c>
       <c r="W39" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -5243,7 +5342,7 @@
         <v>119</v>
       </c>
       <c r="W41" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="X41" t="s">
         <v>380</v>
@@ -5319,6 +5418,9 @@
       <c r="W42" t="s">
         <v>336</v>
       </c>
+      <c r="X42" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -5464,6 +5566,9 @@
       <c r="W44" t="s">
         <v>336</v>
       </c>
+      <c r="X44" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -5749,7 +5854,10 @@
         <v>106</v>
       </c>
       <c r="W48" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X48" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -5820,7 +5928,7 @@
         <v>125</v>
       </c>
       <c r="W49" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
@@ -5891,7 +5999,7 @@
         <v>126</v>
       </c>
       <c r="W50" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
@@ -6036,7 +6144,10 @@
         <v>129</v>
       </c>
       <c r="W52" t="s">
-        <v>413</v>
+        <v>412</v>
+      </c>
+      <c r="X52" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
@@ -6323,7 +6434,10 @@
         <v>133</v>
       </c>
       <c r="W56" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X56" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -6465,7 +6579,7 @@
         <v>136</v>
       </c>
       <c r="W58" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -6610,7 +6724,10 @@
         <v>140</v>
       </c>
       <c r="W60" t="s">
-        <v>416</v>
+        <v>415</v>
+      </c>
+      <c r="X60" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -6752,7 +6869,7 @@
         <v>144</v>
       </c>
       <c r="W62" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
@@ -6823,7 +6940,7 @@
         <v>145</v>
       </c>
       <c r="W63" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="X63" t="s">
         <v>353</v>
@@ -6899,6 +7016,9 @@
       <c r="W64" t="s">
         <v>338</v>
       </c>
+      <c r="X64" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -6968,7 +7088,7 @@
         <v>147</v>
       </c>
       <c r="W65" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
@@ -7184,7 +7304,10 @@
         <v>150</v>
       </c>
       <c r="W68" t="s">
-        <v>420</v>
+        <v>419</v>
+      </c>
+      <c r="X68" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
@@ -7326,7 +7449,7 @@
         <v>152</v>
       </c>
       <c r="W70" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
@@ -7471,7 +7594,10 @@
         <v>154</v>
       </c>
       <c r="W72" t="s">
-        <v>422</v>
+        <v>421</v>
+      </c>
+      <c r="X72" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
@@ -7616,7 +7742,10 @@
         <v>106</v>
       </c>
       <c r="W74" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X74" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
@@ -7905,6 +8034,9 @@
       <c r="W78" t="s">
         <v>318</v>
       </c>
+      <c r="X78" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -8045,7 +8177,7 @@
         <v>113</v>
       </c>
       <c r="W80" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
@@ -8190,7 +8322,10 @@
         <v>133</v>
       </c>
       <c r="W82" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X82" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
@@ -8403,7 +8538,7 @@
         <v>165</v>
       </c>
       <c r="W85" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="X85" t="s">
         <v>377</v>
@@ -8477,7 +8612,10 @@
         <v>129</v>
       </c>
       <c r="W86" t="s">
-        <v>413</v>
+        <v>412</v>
+      </c>
+      <c r="X86" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
@@ -8548,7 +8686,7 @@
         <v>125</v>
       </c>
       <c r="W87" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
@@ -8619,7 +8757,7 @@
         <v>168</v>
       </c>
       <c r="W88" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
@@ -8764,7 +8902,10 @@
         <v>106</v>
       </c>
       <c r="W90" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X90" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
@@ -8835,7 +8976,7 @@
         <v>171</v>
       </c>
       <c r="W91" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
@@ -8977,7 +9118,7 @@
         <v>129</v>
       </c>
       <c r="W93" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X93" t="s">
         <v>384</v>
@@ -9051,7 +9192,10 @@
         <v>175</v>
       </c>
       <c r="W94" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+      <c r="X94" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
@@ -9264,7 +9408,7 @@
         <v>179</v>
       </c>
       <c r="W97" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="X97" t="s">
         <v>366</v>
@@ -9340,6 +9484,9 @@
       <c r="W98" t="s">
         <v>336</v>
       </c>
+      <c r="X98" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
@@ -9409,7 +9556,7 @@
         <v>180</v>
       </c>
       <c r="W99" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
@@ -9480,7 +9627,7 @@
         <v>181</v>
       </c>
       <c r="W100" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.25">
@@ -9625,7 +9772,10 @@
         <v>133</v>
       </c>
       <c r="W102" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X102" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
@@ -9772,6 +9922,9 @@
       <c r="W104" t="s">
         <v>336</v>
       </c>
+      <c r="X104" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
@@ -9912,7 +10065,7 @@
         <v>113</v>
       </c>
       <c r="W106" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
@@ -9983,7 +10136,7 @@
         <v>185</v>
       </c>
       <c r="W107" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="X107" t="s">
         <v>362</v>
@@ -10057,7 +10210,7 @@
         <v>188</v>
       </c>
       <c r="W108" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
@@ -10347,7 +10500,10 @@
         <v>133</v>
       </c>
       <c r="W112" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X112" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
@@ -10560,7 +10716,7 @@
         <v>196</v>
       </c>
       <c r="W115" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="X115" t="s">
         <v>354</v>
@@ -10705,7 +10861,7 @@
         <v>200</v>
       </c>
       <c r="W117" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
@@ -10776,7 +10932,7 @@
         <v>202</v>
       </c>
       <c r="W118" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X118" t="s">
         <v>394</v>
@@ -10850,7 +11006,7 @@
         <v>129</v>
       </c>
       <c r="W119" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="X119" t="s">
         <v>384</v>
@@ -10924,7 +11080,10 @@
         <v>154</v>
       </c>
       <c r="W120" t="s">
-        <v>422</v>
+        <v>421</v>
+      </c>
+      <c r="X120" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
@@ -10995,7 +11154,7 @@
         <v>206</v>
       </c>
       <c r="W121" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
@@ -11066,7 +11225,7 @@
         <v>113</v>
       </c>
       <c r="W122" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
@@ -11137,7 +11296,7 @@
         <v>208</v>
       </c>
       <c r="W123" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="X123" t="s">
         <v>355</v>
@@ -11211,7 +11370,7 @@
         <v>210</v>
       </c>
       <c r="W124" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.25">
@@ -11427,7 +11586,10 @@
         <v>213</v>
       </c>
       <c r="W127" t="s">
-        <v>437</v>
+        <v>436</v>
+      </c>
+      <c r="X127" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.25">
@@ -11930,7 +12092,7 @@
         <v>179</v>
       </c>
       <c r="W134" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="X134" t="s">
         <v>366</v>
@@ -12004,7 +12166,10 @@
         <v>154</v>
       </c>
       <c r="W135" t="s">
-        <v>422</v>
+        <v>421</v>
+      </c>
+      <c r="X135" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="136" spans="1:24" x14ac:dyDescent="0.25">
@@ -12075,7 +12240,7 @@
         <v>125</v>
       </c>
       <c r="W136" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.25">
@@ -12217,7 +12382,7 @@
         <v>226</v>
       </c>
       <c r="W138" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="X138" t="s">
         <v>376</v>
@@ -12362,7 +12527,7 @@
         <v>229</v>
       </c>
       <c r="W140" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="141" spans="1:24" x14ac:dyDescent="0.25">
@@ -12581,7 +12746,10 @@
         <v>232</v>
       </c>
       <c r="W143" t="s">
-        <v>440</v>
+        <v>439</v>
+      </c>
+      <c r="X143" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.25">
@@ -12652,7 +12820,7 @@
         <v>206</v>
       </c>
       <c r="W144" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="145" spans="1:24" x14ac:dyDescent="0.25">
@@ -12794,7 +12962,7 @@
         <v>185</v>
       </c>
       <c r="W146" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="X146" t="s">
         <v>363</v>
@@ -12868,7 +13036,7 @@
         <v>236</v>
       </c>
       <c r="W147" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="148" spans="1:24" x14ac:dyDescent="0.25">
@@ -12939,7 +13107,7 @@
         <v>238</v>
       </c>
       <c r="W148" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="149" spans="1:24" x14ac:dyDescent="0.25">
@@ -13158,7 +13326,10 @@
         <v>111</v>
       </c>
       <c r="W151" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X151" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="152" spans="1:24" x14ac:dyDescent="0.25">
@@ -13229,7 +13400,7 @@
         <v>240</v>
       </c>
       <c r="W152" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="153" spans="1:24" x14ac:dyDescent="0.25">
@@ -13300,7 +13471,7 @@
         <v>113</v>
       </c>
       <c r="W153" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="154" spans="1:24" x14ac:dyDescent="0.25">
@@ -13371,7 +13542,7 @@
         <v>210</v>
       </c>
       <c r="W154" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="X154" t="s">
         <v>356</v>
@@ -13519,7 +13690,10 @@
         <v>133</v>
       </c>
       <c r="W156" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X156" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="157" spans="1:24" x14ac:dyDescent="0.25">
@@ -13877,7 +14051,7 @@
         <v>200</v>
       </c>
       <c r="W161" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="162" spans="1:24" x14ac:dyDescent="0.25">
@@ -13948,7 +14122,7 @@
         <v>202</v>
       </c>
       <c r="W162" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X162" t="s">
         <v>394</v>
@@ -14096,7 +14270,10 @@
         <v>110</v>
       </c>
       <c r="W164" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X164" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="165" spans="1:24" x14ac:dyDescent="0.25">
@@ -14167,7 +14344,7 @@
         <v>125</v>
       </c>
       <c r="W165" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="166" spans="1:24" x14ac:dyDescent="0.25">
@@ -14309,7 +14486,7 @@
         <v>247</v>
       </c>
       <c r="W167" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="X167" t="s">
         <v>375</v>
@@ -14383,7 +14560,7 @@
         <v>248</v>
       </c>
       <c r="W168" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="169" spans="1:24" x14ac:dyDescent="0.25">
@@ -14454,7 +14631,7 @@
         <v>249</v>
       </c>
       <c r="W169" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="170" spans="1:24" x14ac:dyDescent="0.25">
@@ -14599,7 +14776,7 @@
         <v>252</v>
       </c>
       <c r="W171" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X171" t="s">
         <v>378</v>
@@ -14673,7 +14850,10 @@
         <v>106</v>
       </c>
       <c r="W172" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X172" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="173" spans="1:24" x14ac:dyDescent="0.25">
@@ -14815,7 +14995,7 @@
         <v>113</v>
       </c>
       <c r="W174" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="175" spans="1:24" x14ac:dyDescent="0.25">
@@ -14886,7 +15066,7 @@
         <v>254</v>
       </c>
       <c r="W175" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="X175" t="s">
         <v>359</v>
@@ -14960,7 +15140,7 @@
         <v>256</v>
       </c>
       <c r="W176" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="177" spans="1:24" x14ac:dyDescent="0.25">
@@ -15031,7 +15211,7 @@
         <v>229</v>
       </c>
       <c r="W177" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="178" spans="1:24" x14ac:dyDescent="0.25">
@@ -15105,7 +15285,7 @@
         <v>347</v>
       </c>
       <c r="X178" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="179" spans="1:24" x14ac:dyDescent="0.25">
@@ -15176,7 +15356,7 @@
         <v>252</v>
       </c>
       <c r="W179" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X179" t="s">
         <v>378</v>
@@ -15250,7 +15430,10 @@
         <v>260</v>
       </c>
       <c r="W180" t="s">
-        <v>451</v>
+        <v>450</v>
+      </c>
+      <c r="X180" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="181" spans="1:24" x14ac:dyDescent="0.25">
@@ -15392,7 +15575,7 @@
         <v>126</v>
       </c>
       <c r="W182" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="183" spans="1:24" x14ac:dyDescent="0.25">
@@ -15463,7 +15646,7 @@
         <v>247</v>
       </c>
       <c r="W183" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="X183" t="s">
         <v>375</v>
@@ -15611,7 +15794,10 @@
         <v>111</v>
       </c>
       <c r="W185" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X185" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="186" spans="1:24" x14ac:dyDescent="0.25">
@@ -15682,7 +15868,7 @@
         <v>108</v>
       </c>
       <c r="W186" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="187" spans="1:24" x14ac:dyDescent="0.25">
@@ -15753,7 +15939,7 @@
         <v>152</v>
       </c>
       <c r="W187" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="188" spans="1:24" x14ac:dyDescent="0.25">
@@ -15824,7 +16010,7 @@
         <v>254</v>
       </c>
       <c r="W188" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="X188" t="s">
         <v>359</v>
@@ -15969,7 +16155,7 @@
         <v>249</v>
       </c>
       <c r="W190" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="191" spans="1:24" x14ac:dyDescent="0.25">
@@ -16188,7 +16374,10 @@
         <v>110</v>
       </c>
       <c r="W193" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X193" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="194" spans="1:24" x14ac:dyDescent="0.25">
@@ -16259,7 +16448,7 @@
         <v>265</v>
       </c>
       <c r="W194" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="195" spans="1:24" x14ac:dyDescent="0.25">
@@ -16401,7 +16590,7 @@
         <v>247</v>
       </c>
       <c r="W196" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="X196" t="s">
         <v>375</v>
@@ -16475,7 +16664,7 @@
         <v>256</v>
       </c>
       <c r="W197" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="198" spans="1:24" x14ac:dyDescent="0.25">
@@ -16546,7 +16735,7 @@
         <v>200</v>
       </c>
       <c r="W198" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="199" spans="1:24" x14ac:dyDescent="0.25">
@@ -16617,7 +16806,7 @@
         <v>202</v>
       </c>
       <c r="W199" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X199" t="s">
         <v>394</v>
@@ -16691,7 +16880,7 @@
         <v>252</v>
       </c>
       <c r="W200" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X200" t="s">
         <v>378</v>
@@ -16765,7 +16954,10 @@
         <v>133</v>
       </c>
       <c r="W201" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X201" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="202" spans="1:24" x14ac:dyDescent="0.25">
@@ -17123,7 +17315,7 @@
         <v>249</v>
       </c>
       <c r="W206" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="207" spans="1:24" x14ac:dyDescent="0.25">
@@ -17342,7 +17534,10 @@
         <v>111</v>
       </c>
       <c r="W209" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X209" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="210" spans="1:24" x14ac:dyDescent="0.25">
@@ -17413,7 +17608,7 @@
         <v>265</v>
       </c>
       <c r="W210" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="211" spans="1:24" x14ac:dyDescent="0.25">
@@ -17555,7 +17750,7 @@
         <v>272</v>
       </c>
       <c r="W212" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="X212" t="s">
         <v>369</v>
@@ -17629,7 +17824,10 @@
         <v>133</v>
       </c>
       <c r="W213" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X213" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="214" spans="1:24" x14ac:dyDescent="0.25">
@@ -17700,7 +17898,7 @@
         <v>273</v>
       </c>
       <c r="W214" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="215" spans="1:24" x14ac:dyDescent="0.25">
@@ -17987,7 +18185,7 @@
         <v>200</v>
       </c>
       <c r="W218" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="219" spans="1:24" x14ac:dyDescent="0.25">
@@ -18058,10 +18256,10 @@
         <v>274</v>
       </c>
       <c r="W219" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="X219" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="220" spans="1:24" x14ac:dyDescent="0.25">
@@ -18206,7 +18404,10 @@
         <v>111</v>
       </c>
       <c r="W221" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X221" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="222" spans="1:24" x14ac:dyDescent="0.25">
@@ -18348,7 +18549,7 @@
         <v>152</v>
       </c>
       <c r="W223" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="224" spans="1:24" x14ac:dyDescent="0.25">
@@ -18419,7 +18620,7 @@
         <v>247</v>
       </c>
       <c r="W224" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="X224" t="s">
         <v>375</v>
@@ -18564,7 +18765,7 @@
         <v>249</v>
       </c>
       <c r="W226" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="227" spans="1:24" x14ac:dyDescent="0.25">
@@ -18783,7 +18984,10 @@
         <v>110</v>
       </c>
       <c r="W229" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X229" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="230" spans="1:24" x14ac:dyDescent="0.25">
@@ -18854,7 +19058,7 @@
         <v>108</v>
       </c>
       <c r="W230" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="231" spans="1:24" x14ac:dyDescent="0.25">
@@ -18925,7 +19129,7 @@
         <v>126</v>
       </c>
       <c r="W231" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="232" spans="1:24" x14ac:dyDescent="0.25">
@@ -18996,7 +19200,7 @@
         <v>254</v>
       </c>
       <c r="W232" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="X232" t="s">
         <v>359</v>
@@ -19141,7 +19345,7 @@
         <v>249</v>
       </c>
       <c r="W234" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="235" spans="1:24" x14ac:dyDescent="0.25">
@@ -19212,7 +19416,7 @@
         <v>274</v>
       </c>
       <c r="W235" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="236" spans="1:24" x14ac:dyDescent="0.25">
@@ -19357,7 +19561,10 @@
         <v>281</v>
       </c>
       <c r="W237" t="s">
-        <v>456</v>
+        <v>455</v>
+      </c>
+      <c r="X237" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="238" spans="1:24" x14ac:dyDescent="0.25">
@@ -19646,6 +19853,9 @@
       <c r="W241" t="s">
         <v>336</v>
       </c>
+      <c r="X241" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="242" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
@@ -19715,7 +19925,7 @@
         <v>265</v>
       </c>
       <c r="W242" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="243" spans="1:24" x14ac:dyDescent="0.25">
@@ -20002,7 +20212,7 @@
         <v>188</v>
       </c>
       <c r="W246" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="247" spans="1:24" x14ac:dyDescent="0.25">
@@ -20073,7 +20283,7 @@
         <v>202</v>
       </c>
       <c r="W247" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X247" t="s">
         <v>394</v>
@@ -20147,7 +20357,7 @@
         <v>179</v>
       </c>
       <c r="W248" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="X248" t="s">
         <v>366</v>
@@ -20221,7 +20431,10 @@
         <v>154</v>
       </c>
       <c r="W249" t="s">
-        <v>422</v>
+        <v>421</v>
+      </c>
+      <c r="X249" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="250" spans="1:24" x14ac:dyDescent="0.25">
@@ -20292,7 +20505,7 @@
         <v>285</v>
       </c>
       <c r="W250" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="251" spans="1:24" x14ac:dyDescent="0.25">
@@ -20363,7 +20576,7 @@
         <v>286</v>
       </c>
       <c r="W251" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="252" spans="1:24" x14ac:dyDescent="0.25">
@@ -20434,7 +20647,7 @@
         <v>210</v>
       </c>
       <c r="W252" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="X252" t="s">
         <v>356</v>
@@ -20579,7 +20792,7 @@
         <v>289</v>
       </c>
       <c r="W254" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="255" spans="1:24" x14ac:dyDescent="0.25">
@@ -20724,7 +20937,7 @@
         <v>252</v>
       </c>
       <c r="W256" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X256" t="s">
         <v>378</v>
@@ -20798,7 +21011,10 @@
         <v>290</v>
       </c>
       <c r="W257" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="X257" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="258" spans="1:24" x14ac:dyDescent="0.25">
@@ -21011,7 +21227,7 @@
         <v>293</v>
       </c>
       <c r="W260" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="X260" t="s">
         <v>358</v>
@@ -21085,7 +21301,7 @@
         <v>294</v>
       </c>
       <c r="W261" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="262" spans="1:24" x14ac:dyDescent="0.25">
@@ -21156,7 +21372,7 @@
         <v>248</v>
       </c>
       <c r="W262" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="263" spans="1:24" x14ac:dyDescent="0.25">
@@ -21227,7 +21443,7 @@
         <v>296</v>
       </c>
       <c r="W263" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="X263" t="s">
         <v>392</v>
@@ -21375,7 +21591,10 @@
         <v>106</v>
       </c>
       <c r="W265" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X265" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="266" spans="1:24" x14ac:dyDescent="0.25">
@@ -21446,7 +21665,7 @@
         <v>125</v>
       </c>
       <c r="W266" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="267" spans="1:24" x14ac:dyDescent="0.25">
@@ -21517,7 +21736,7 @@
         <v>126</v>
       </c>
       <c r="W267" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="268" spans="1:24" x14ac:dyDescent="0.25">
@@ -21588,7 +21807,7 @@
         <v>247</v>
       </c>
       <c r="W268" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="X268" t="s">
         <v>375</v>
@@ -21733,7 +21952,7 @@
         <v>200</v>
       </c>
       <c r="W270" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="271" spans="1:24" x14ac:dyDescent="0.25">
@@ -21952,7 +22171,10 @@
         <v>290</v>
       </c>
       <c r="W273" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="X273" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="274" spans="1:24" x14ac:dyDescent="0.25">
@@ -22023,7 +22245,7 @@
         <v>147</v>
       </c>
       <c r="W274" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="275" spans="1:24" x14ac:dyDescent="0.25">
@@ -22165,7 +22387,7 @@
         <v>210</v>
       </c>
       <c r="W276" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="X276" t="s">
         <v>356</v>
@@ -22239,7 +22461,7 @@
         <v>299</v>
       </c>
       <c r="W277" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="278" spans="1:24" x14ac:dyDescent="0.25">
@@ -22310,7 +22532,7 @@
         <v>188</v>
       </c>
       <c r="W278" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="279" spans="1:24" x14ac:dyDescent="0.25">
@@ -22455,7 +22677,7 @@
         <v>252</v>
       </c>
       <c r="W280" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X280" t="s">
         <v>378</v>
@@ -22529,7 +22751,10 @@
         <v>213</v>
       </c>
       <c r="W281" t="s">
-        <v>437</v>
+        <v>436</v>
+      </c>
+      <c r="X281" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="282" spans="1:24" x14ac:dyDescent="0.25">
@@ -22600,7 +22825,7 @@
         <v>265</v>
       </c>
       <c r="W282" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="283" spans="1:24" x14ac:dyDescent="0.25">
@@ -22887,7 +23112,7 @@
         <v>200</v>
       </c>
       <c r="W286" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="287" spans="1:24" x14ac:dyDescent="0.25">
@@ -22958,10 +23183,10 @@
         <v>301</v>
       </c>
       <c r="W287" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="X287" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="288" spans="1:24" x14ac:dyDescent="0.25">
@@ -23106,10 +23331,10 @@
         <v>110</v>
       </c>
       <c r="W289" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="X289" t="s">
-        <v>396</v>
+        <v>478</v>
       </c>
     </row>
     <row r="290" spans="1:24" x14ac:dyDescent="0.25">
@@ -23325,7 +23550,10 @@
         <v>111</v>
       </c>
       <c r="W292" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X292" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="293" spans="1:24" x14ac:dyDescent="0.25">
@@ -23396,7 +23624,7 @@
         <v>285</v>
       </c>
       <c r="W293" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="294" spans="1:24" x14ac:dyDescent="0.25">
@@ -23683,7 +23911,7 @@
         <v>188</v>
       </c>
       <c r="W297" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="298" spans="1:24" x14ac:dyDescent="0.25">
@@ -23754,7 +23982,7 @@
         <v>305</v>
       </c>
       <c r="W298" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="X298" t="s">
         <v>393</v>
@@ -23904,6 +24132,9 @@
       <c r="W300" t="s">
         <v>318</v>
       </c>
+      <c r="X300" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="301" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
@@ -23973,7 +24204,7 @@
         <v>273</v>
       </c>
       <c r="W301" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="302" spans="1:24" x14ac:dyDescent="0.25">
@@ -24044,7 +24275,7 @@
         <v>113</v>
       </c>
       <c r="W302" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="303" spans="1:24" x14ac:dyDescent="0.25">
@@ -24479,7 +24710,10 @@
         <v>110</v>
       </c>
       <c r="W308" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X308" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="309" spans="1:24" x14ac:dyDescent="0.25">
@@ -24621,7 +24855,7 @@
         <v>113</v>
       </c>
       <c r="W310" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="311" spans="1:24" x14ac:dyDescent="0.25">
@@ -24692,7 +24926,7 @@
         <v>188</v>
       </c>
       <c r="W311" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="X311" t="s">
         <v>357</v>
@@ -24837,7 +25071,7 @@
         <v>200</v>
       </c>
       <c r="W313" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="314" spans="1:24" x14ac:dyDescent="0.25">
@@ -24908,7 +25142,7 @@
         <v>202</v>
       </c>
       <c r="W314" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X314" t="s">
         <v>394</v>
@@ -25056,7 +25290,10 @@
         <v>260</v>
       </c>
       <c r="W316" t="s">
-        <v>451</v>
+        <v>450</v>
+      </c>
+      <c r="X316" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="317" spans="1:24" x14ac:dyDescent="0.25">
@@ -25343,7 +25580,10 @@
         <v>110</v>
       </c>
       <c r="W320" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X320" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="321" spans="1:24" x14ac:dyDescent="0.25">
@@ -25556,7 +25796,7 @@
         <v>210</v>
       </c>
       <c r="W323" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="X323" t="s">
         <v>356</v>
@@ -25701,7 +25941,7 @@
         <v>200</v>
       </c>
       <c r="W325" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="326" spans="1:24" x14ac:dyDescent="0.25">
@@ -25772,7 +26012,7 @@
         <v>202</v>
       </c>
       <c r="W326" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X326" t="s">
         <v>394</v>
@@ -25920,7 +26160,10 @@
         <v>111</v>
       </c>
       <c r="W328" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X328" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="329" spans="1:24" x14ac:dyDescent="0.25">
@@ -25991,7 +26234,7 @@
         <v>285</v>
       </c>
       <c r="W329" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="330" spans="1:24" x14ac:dyDescent="0.25">
@@ -26133,7 +26376,7 @@
         <v>247</v>
       </c>
       <c r="W331" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="X331" t="s">
         <v>375</v>
@@ -26278,7 +26521,7 @@
         <v>188</v>
       </c>
       <c r="W333" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="334" spans="1:24" x14ac:dyDescent="0.25">
@@ -26499,6 +26742,9 @@
       <c r="W336" t="s">
         <v>318</v>
       </c>
+      <c r="X336" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="337" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
@@ -26568,7 +26814,7 @@
         <v>273</v>
       </c>
       <c r="W337" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="338" spans="1:24" x14ac:dyDescent="0.25">
@@ -26639,7 +26885,7 @@
         <v>113</v>
       </c>
       <c r="W338" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="339" spans="1:24" x14ac:dyDescent="0.25">
@@ -26926,7 +27172,7 @@
         <v>296</v>
       </c>
       <c r="W342" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="X342" t="s">
         <v>392</v>
@@ -27074,7 +27320,7 @@
         <v>125</v>
       </c>
       <c r="W344" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="345" spans="1:24" x14ac:dyDescent="0.25">
@@ -27216,7 +27462,7 @@
         <v>226</v>
       </c>
       <c r="W346" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="X346" t="s">
         <v>376</v>
@@ -27361,7 +27607,7 @@
         <v>200</v>
       </c>
       <c r="W348" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="349" spans="1:24" x14ac:dyDescent="0.25">
@@ -27580,7 +27826,10 @@
         <v>111</v>
       </c>
       <c r="W351" t="s">
-        <v>406</v>
+        <v>405</v>
+      </c>
+      <c r="X351" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="352" spans="1:24" x14ac:dyDescent="0.25">
@@ -27793,7 +28042,7 @@
         <v>307</v>
       </c>
       <c r="W354" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="X354" t="s">
         <v>364</v>
@@ -27938,7 +28187,7 @@
         <v>188</v>
       </c>
       <c r="W356" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="357" spans="1:24" x14ac:dyDescent="0.25">
@@ -28009,7 +28258,7 @@
         <v>202</v>
       </c>
       <c r="W357" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X357" t="s">
         <v>394</v>
@@ -28157,7 +28406,10 @@
         <v>110</v>
       </c>
       <c r="W359" t="s">
-        <v>405</v>
+        <v>404</v>
+      </c>
+      <c r="X359" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="360" spans="1:24" x14ac:dyDescent="0.25">
@@ -28228,7 +28480,7 @@
         <v>180</v>
       </c>
       <c r="W360" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="361" spans="1:24" x14ac:dyDescent="0.25">
@@ -28515,7 +28767,7 @@
         <v>200</v>
       </c>
       <c r="W364" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="365" spans="1:24" x14ac:dyDescent="0.25">
@@ -28586,7 +28838,7 @@
         <v>296</v>
       </c>
       <c r="W365" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="X365" t="s">
         <v>392</v>
@@ -28660,7 +28912,7 @@
         <v>252</v>
       </c>
       <c r="W366" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X366" t="s">
         <v>378</v>
@@ -28736,6 +28988,9 @@
       <c r="W367" t="s">
         <v>345</v>
       </c>
+      <c r="X367" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="368" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
@@ -28805,7 +29060,7 @@
         <v>125</v>
       </c>
       <c r="W368" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="369" spans="1:24" x14ac:dyDescent="0.25">
@@ -29018,7 +29273,7 @@
         <v>200</v>
       </c>
       <c r="W371" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="372" spans="1:24" x14ac:dyDescent="0.25">
@@ -29089,7 +29344,7 @@
         <v>202</v>
       </c>
       <c r="W372" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X372" t="s">
         <v>394</v>
@@ -29163,7 +29418,7 @@
         <v>265</v>
       </c>
       <c r="W373" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="374" spans="1:24" x14ac:dyDescent="0.25">
@@ -29450,7 +29705,7 @@
         <v>200</v>
       </c>
       <c r="W377" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="378" spans="1:24" x14ac:dyDescent="0.25">
@@ -29669,7 +29924,10 @@
         <v>106</v>
       </c>
       <c r="W380" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="X380" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="381" spans="1:24" x14ac:dyDescent="0.25">
@@ -29740,7 +29998,7 @@
         <v>125</v>
       </c>
       <c r="W381" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="382" spans="1:24" x14ac:dyDescent="0.25">
@@ -30027,7 +30285,7 @@
         <v>229</v>
       </c>
       <c r="W385" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="386" spans="1:24" x14ac:dyDescent="0.25">
@@ -30098,7 +30356,7 @@
         <v>305</v>
       </c>
       <c r="W386" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="X386" t="s">
         <v>393</v>
@@ -30172,7 +30430,7 @@
         <v>252</v>
       </c>
       <c r="W387" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="X387" t="s">
         <v>378</v>
@@ -30246,7 +30504,10 @@
         <v>290</v>
       </c>
       <c r="W388" t="s">
-        <v>460</v>
+        <v>459</v>
+      </c>
+      <c r="X388" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="389" spans="1:24" x14ac:dyDescent="0.25">
@@ -30601,7 +30862,7 @@
         <v>200</v>
       </c>
       <c r="W393" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="394" spans="1:24" x14ac:dyDescent="0.25">
@@ -30672,10 +30933,10 @@
         <v>301</v>
       </c>
       <c r="W394" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="X394" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="395" spans="1:24" x14ac:dyDescent="0.25">
@@ -30817,7 +31078,7 @@
         <v>310</v>
       </c>
       <c r="W396" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="397" spans="1:24" x14ac:dyDescent="0.25">
@@ -30962,7 +31223,7 @@
         <v>265</v>
       </c>
       <c r="W398" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="399" spans="1:24" x14ac:dyDescent="0.25">
@@ -31104,7 +31365,7 @@
         <v>200</v>
       </c>
       <c r="W400" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="401" spans="1:24" x14ac:dyDescent="0.25">
@@ -31175,7 +31436,7 @@
         <v>202</v>
       </c>
       <c r="W401" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X401" t="s">
         <v>394</v>
@@ -31249,7 +31510,7 @@
         <v>312</v>
       </c>
       <c r="W402" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="X402" t="s">
         <v>368</v>
@@ -31325,6 +31586,9 @@
       <c r="W403" t="s">
         <v>318</v>
       </c>
+      <c r="X403" t="s">
+        <v>479</v>
+      </c>
     </row>
     <row r="404" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
@@ -31394,7 +31658,7 @@
         <v>240</v>
       </c>
       <c r="W404" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="405" spans="1:24" x14ac:dyDescent="0.25">
@@ -31678,7 +31942,7 @@
         <v>200</v>
       </c>
       <c r="W408" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="409" spans="1:24" x14ac:dyDescent="0.25">
@@ -31749,7 +32013,7 @@
         <v>202</v>
       </c>
       <c r="W409" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="X409" t="s">
         <v>394</v>
@@ -31965,7 +32229,7 @@
         <v>289</v>
       </c>
       <c r="W412" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="413" spans="1:24" x14ac:dyDescent="0.25">
@@ -32036,7 +32300,7 @@
         <v>313</v>
       </c>
       <c r="W413" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="X413" t="s">
         <v>388</v>
@@ -32110,7 +32374,7 @@
         <v>229</v>
       </c>
       <c r="W414" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="415" spans="1:24" x14ac:dyDescent="0.25">
@@ -32181,7 +32445,7 @@
         <v>305</v>
       </c>
       <c r="W415" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="X415" t="s">
         <v>393</v>
@@ -32545,7 +32809,10 @@
         <v>133</v>
       </c>
       <c r="W420" t="s">
-        <v>414</v>
+        <v>413</v>
+      </c>
+      <c r="X420" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="421" spans="1:24" x14ac:dyDescent="0.25">
@@ -32616,7 +32883,7 @@
         <v>125</v>
       </c>
       <c r="W421" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="422" spans="1:24" x14ac:dyDescent="0.25">
@@ -32687,7 +32954,7 @@
         <v>265</v>
       </c>
       <c r="W422" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="423" spans="1:24" x14ac:dyDescent="0.25">
@@ -32834,6 +33101,9 @@
       <c r="W424" t="s">
         <v>336</v>
       </c>
+      <c r="X424" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="425" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
@@ -33050,6 +33320,9 @@
       <c r="W427" t="s">
         <v>349</v>
       </c>
+      <c r="X427" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="428" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
@@ -33264,7 +33537,10 @@
         <v>68</v>
       </c>
       <c r="W430" t="s">
-        <v>401</v>
+        <v>400</v>
+      </c>
+      <c r="X430" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="431" spans="1:24" x14ac:dyDescent="0.25">
@@ -33483,7 +33759,7 @@
         <v>374</v>
       </c>
       <c r="X433" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More description added to treatment3
</commit_message>
<xml_diff>
--- a/cleaned_animal_disease_prediction.xlsx
+++ b/cleaned_animal_disease_prediction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abbey\Documents\finalyear_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2CD708-33AB-4CD6-A452-CB47881CD66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D2681F-59A4-4401-BA0E-F5CEF4B75BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="cleaned_animal_disease_predicti" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cleaned_animal_disease_predicti!$A$1:$W$433</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cleaned_animal_disease_predicti!$A$1:$W$434</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8883" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8925" uniqueCount="504">
   <si>
     <t>species</t>
   </si>
@@ -1499,6 +1499,42 @@
   </si>
   <si>
     <t>Ringworm (dermatophytosis) is a fungal infection of the skin, hair, or claws—not caused by a worm.</t>
+  </si>
+  <si>
+    <t>CAE is a chronic viral disease caused by a lentivirus (small ruminant lentivirus group), affecting goats worldwide. It manifests in multiple forms, primarily targeting joints, the nervous system, udder, and lungs.</t>
+  </si>
+  <si>
+    <t>CCPP is a highly contagious respiratory disease in goats caused by the bacterium Mycoplasma capricolum subspecies capripneumoniae. It is characterized by severe lung inflammation and pleural fluid buildup, leading to high mortality if untreated.</t>
+  </si>
+  <si>
+    <t>Caprine Respiratory Disease is a common, often multifactorial illness affecting the respiratory system of goats, caused by a combination of bacteria, viruses, parasites, and environmental stressors.</t>
+  </si>
+  <si>
+    <t>Caprine Viral Arthritis is a chronic viral disease in goats caused by the Caprine Arthritis-Encephalitis Virus (CAEV), a retrovirus. It primarily affects the joints, udder, and nervous system, leading to progressive debilitation.</t>
+  </si>
+  <si>
+    <t>Caseous Lymphadenitis is a chronic bacterial infection caused by Corynebacterium pseudotuberculosis. It is characterized by abscess formation in lymph nodes (especially head, neck, and internal organs) and is highly contagious among goats and sheep.</t>
+  </si>
+  <si>
+    <t>Coccidiosis is a parasitic disease caused by protozoa of the Eimeria genus, which infect the intestinal lining of goats. It primarily affects young kids (2–6 months old) and is a major cause of diarrhea and poor growth in herds.</t>
+  </si>
+  <si>
+    <t>Foot and Mouth Disease is a highly contagious viral disease caused by the Aphthovirus (Picornaviridae family). It affects cloven-hoofed animals, including goats, cattle, and pigs.</t>
+  </si>
+  <si>
+    <t>Gastrointestinal (GI) infections in goats are digestive tract disorders caused by bacteria, viruses, parasites, or dietary issues, leading to diarrhea, dehydration, and weight loss. </t>
+  </si>
+  <si>
+    <t>Giardiasis is a protozoal parasitic infection caused by Giardia duodenalis (also called Giardia lamblia), affecting the small intestine of goats.</t>
+  </si>
+  <si>
+    <t>Goat pox is a highly contagious viral disease caused by Capripoxvirus, affecting goats (and sometimes sheep).</t>
+  </si>
+  <si>
+    <t>Pneumonia in goats is a respiratory disease characterized by inflammation of the lungs, often caused by bacterial, viral, or parasitic infections, as well as environmental stressors.</t>
+  </si>
+  <si>
+    <t>It primarily affects calves (3 weeks to 6 months old) but can also occur in stressed or immunocompromised adult cattle. </t>
   </si>
 </sst>
 </file>
@@ -2347,16 +2383,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X433"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:X434"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="W436" sqref="W436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="22" max="22" width="55.85546875" customWidth="1"/>
-    <col min="23" max="23" width="143.42578125" customWidth="1"/>
+    <col min="23" max="23" width="216.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -2433,7 +2470,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2507,7 +2544,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -2581,7 +2618,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2652,7 +2689,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +2763,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2800,7 +2837,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -2871,7 +2908,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2945,7 +2982,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3019,7 +3056,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3093,7 +3130,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -3164,7 +3201,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3238,7 +3275,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -3312,7 +3349,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3386,7 +3423,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3457,7 +3494,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -3528,7 +3565,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -3602,7 +3639,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -3676,7 +3713,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3750,7 +3787,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -3821,7 +3858,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -3895,7 +3932,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -3966,7 +4003,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -4037,7 +4074,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -4111,7 +4148,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -4185,7 +4222,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -4256,7 +4293,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -4330,7 +4367,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -4404,7 +4441,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -4475,7 +4512,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -4549,7 +4586,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -4623,7 +4660,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -4694,7 +4731,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -4768,7 +4805,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -4842,7 +4879,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>57</v>
       </c>
@@ -4913,7 +4950,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -4984,7 +5021,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>22</v>
       </c>
@@ -5058,7 +5095,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -5132,7 +5169,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>57</v>
       </c>
@@ -5203,7 +5240,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -5274,7 +5311,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -5348,7 +5385,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -5422,7 +5459,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>22</v>
       </c>
@@ -5496,7 +5533,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>33</v>
       </c>
@@ -5570,7 +5607,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>57</v>
       </c>
@@ -5641,7 +5678,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -5712,7 +5749,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -5786,7 +5823,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>33</v>
       </c>
@@ -5860,7 +5897,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -5931,7 +5968,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -6002,7 +6039,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>22</v>
       </c>
@@ -6076,7 +6113,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>33</v>
       </c>
@@ -6150,7 +6187,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -6221,7 +6258,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>42</v>
       </c>
@@ -6292,7 +6329,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>22</v>
       </c>
@@ -6366,7 +6403,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>33</v>
       </c>
@@ -6440,7 +6477,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -6511,7 +6548,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>42</v>
       </c>
@@ -6582,7 +6619,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>22</v>
       </c>
@@ -6656,7 +6693,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>33</v>
       </c>
@@ -6730,7 +6767,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -6801,7 +6838,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -6872,7 +6909,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>22</v>
       </c>
@@ -6946,7 +6983,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>33</v>
       </c>
@@ -7020,7 +7057,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>57</v>
       </c>
@@ -7091,7 +7128,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>42</v>
       </c>
@@ -7161,8 +7198,11 @@
       <c r="W66" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X66" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>22</v>
       </c>
@@ -7236,7 +7276,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>33</v>
       </c>
@@ -7310,7 +7350,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>57</v>
       </c>
@@ -7381,7 +7421,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>42</v>
       </c>
@@ -7452,7 +7492,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>22</v>
       </c>
@@ -7526,7 +7566,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -7600,7 +7640,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>22</v>
       </c>
@@ -7674,7 +7714,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>33</v>
       </c>
@@ -7748,7 +7788,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>57</v>
       </c>
@@ -7819,7 +7859,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>42</v>
       </c>
@@ -7890,7 +7930,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>22</v>
       </c>
@@ -7964,7 +8004,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>33</v>
       </c>
@@ -8038,7 +8078,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>57</v>
       </c>
@@ -8109,7 +8149,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -8180,7 +8220,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>22</v>
       </c>
@@ -8254,7 +8294,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>33</v>
       </c>
@@ -8328,7 +8368,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>57</v>
       </c>
@@ -8399,7 +8439,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>42</v>
       </c>
@@ -8470,7 +8510,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -8544,7 +8584,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>33</v>
       </c>
@@ -8618,7 +8658,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>57</v>
       </c>
@@ -8689,7 +8729,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -8760,7 +8800,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>22</v>
       </c>
@@ -8834,7 +8874,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>33</v>
       </c>
@@ -8908,7 +8948,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>57</v>
       </c>
@@ -8979,7 +9019,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>42</v>
       </c>
@@ -9050,7 +9090,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>22</v>
       </c>
@@ -9124,7 +9164,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>33</v>
       </c>
@@ -9198,7 +9238,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>57</v>
       </c>
@@ -9269,7 +9309,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>42</v>
       </c>
@@ -9339,8 +9379,11 @@
       <c r="W96" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X96" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>22</v>
       </c>
@@ -9414,7 +9457,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>33</v>
       </c>
@@ -9488,7 +9531,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>57</v>
       </c>
@@ -9630,7 +9673,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>22</v>
       </c>
@@ -9704,7 +9747,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>33</v>
       </c>
@@ -9778,7 +9821,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>22</v>
       </c>
@@ -9852,7 +9895,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>33</v>
       </c>
@@ -9926,7 +9969,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>57</v>
       </c>
@@ -9997,7 +10040,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>42</v>
       </c>
@@ -10068,7 +10111,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>183</v>
       </c>
@@ -10142,7 +10185,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>186</v>
       </c>
@@ -10213,7 +10256,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>189</v>
       </c>
@@ -10283,8 +10326,11 @@
       <c r="W109" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X109" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>192</v>
       </c>
@@ -10358,7 +10404,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>22</v>
       </c>
@@ -10432,7 +10478,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -10506,7 +10552,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>57</v>
       </c>
@@ -10577,7 +10623,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>42</v>
       </c>
@@ -10648,7 +10694,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>183</v>
       </c>
@@ -10722,7 +10768,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>186</v>
       </c>
@@ -10793,7 +10839,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>189</v>
       </c>
@@ -10863,8 +10909,11 @@
       <c r="W117" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X117" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>192</v>
       </c>
@@ -10938,7 +10987,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>22</v>
       </c>
@@ -11012,7 +11061,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -11086,7 +11135,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>57</v>
       </c>
@@ -11157,7 +11206,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>42</v>
       </c>
@@ -11228,7 +11277,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>183</v>
       </c>
@@ -11302,7 +11351,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>186</v>
       </c>
@@ -11373,7 +11422,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>189</v>
       </c>
@@ -11443,8 +11492,11 @@
       <c r="W125" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X125" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>22</v>
       </c>
@@ -11518,7 +11570,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>33</v>
       </c>
@@ -11592,7 +11644,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>57</v>
       </c>
@@ -11663,7 +11715,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>42</v>
       </c>
@@ -11734,7 +11786,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>183</v>
       </c>
@@ -11808,7 +11860,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>186</v>
       </c>
@@ -11879,7 +11931,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>189</v>
       </c>
@@ -11949,8 +12001,11 @@
       <c r="W132" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X132" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>192</v>
       </c>
@@ -12024,7 +12079,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>22</v>
       </c>
@@ -12098,7 +12153,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>33</v>
       </c>
@@ -12172,7 +12227,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>57</v>
       </c>
@@ -12243,7 +12298,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>42</v>
       </c>
@@ -12314,7 +12369,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>183</v>
       </c>
@@ -12388,7 +12443,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>186</v>
       </c>
@@ -12459,7 +12514,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>189</v>
       </c>
@@ -12529,8 +12584,11 @@
       <c r="W140" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X140" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="141" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>192</v>
       </c>
@@ -12604,7 +12662,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>22</v>
       </c>
@@ -12678,7 +12736,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>33</v>
       </c>
@@ -12752,7 +12810,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>57</v>
       </c>
@@ -12823,7 +12881,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>42</v>
       </c>
@@ -12894,7 +12952,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>183</v>
       </c>
@@ -12968,7 +13026,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>186</v>
       </c>
@@ -13039,7 +13097,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>189</v>
       </c>
@@ -13109,8 +13167,11 @@
       <c r="W148" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X148" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>192</v>
       </c>
@@ -13184,7 +13245,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>22</v>
       </c>
@@ -13258,7 +13319,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>33</v>
       </c>
@@ -13332,7 +13393,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>57</v>
       </c>
@@ -13403,7 +13464,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>42</v>
       </c>
@@ -13474,7 +13535,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>183</v>
       </c>
@@ -13548,7 +13609,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>22</v>
       </c>
@@ -13622,7 +13683,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>33</v>
       </c>
@@ -13696,7 +13757,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>57</v>
       </c>
@@ -13767,7 +13828,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -13838,7 +13899,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>183</v>
       </c>
@@ -13912,7 +13973,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>186</v>
       </c>
@@ -13983,7 +14044,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>189</v>
       </c>
@@ -14053,8 +14114,11 @@
       <c r="W161" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X161" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="162" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>192</v>
       </c>
@@ -14128,7 +14192,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>22</v>
       </c>
@@ -14202,7 +14266,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>33</v>
       </c>
@@ -14276,7 +14340,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>57</v>
       </c>
@@ -14347,7 +14411,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>42</v>
       </c>
@@ -14418,7 +14482,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>183</v>
       </c>
@@ -14492,7 +14556,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>186</v>
       </c>
@@ -14563,7 +14627,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>189</v>
       </c>
@@ -14633,8 +14697,11 @@
       <c r="W169" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X169" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="170" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>192</v>
       </c>
@@ -14708,7 +14775,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>22</v>
       </c>
@@ -14782,7 +14849,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>33</v>
       </c>
@@ -14856,7 +14923,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>57</v>
       </c>
@@ -14927,7 +14994,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>42</v>
       </c>
@@ -14998,7 +15065,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>183</v>
       </c>
@@ -15072,7 +15139,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>186</v>
       </c>
@@ -15143,7 +15210,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>189</v>
       </c>
@@ -15213,8 +15280,11 @@
       <c r="W177" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X177" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="178" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>192</v>
       </c>
@@ -15288,7 +15358,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>22</v>
       </c>
@@ -15362,7 +15432,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>33</v>
       </c>
@@ -15436,7 +15506,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>57</v>
       </c>
@@ -15507,7 +15577,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>42</v>
       </c>
@@ -15578,7 +15648,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -15652,7 +15722,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>22</v>
       </c>
@@ -15726,7 +15796,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>33</v>
       </c>
@@ -15800,7 +15870,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>57</v>
       </c>
@@ -15871,7 +15941,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>42</v>
       </c>
@@ -15942,7 +16012,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>183</v>
       </c>
@@ -16016,7 +16086,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>186</v>
       </c>
@@ -16087,7 +16157,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
@@ -16157,8 +16227,11 @@
       <c r="W190" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X190" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="191" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>192</v>
       </c>
@@ -16232,7 +16305,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>22</v>
       </c>
@@ -16306,7 +16379,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>33</v>
       </c>
@@ -16380,7 +16453,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>57</v>
       </c>
@@ -16451,7 +16524,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>42</v>
       </c>
@@ -16522,7 +16595,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>183</v>
       </c>
@@ -16596,7 +16669,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>186</v>
       </c>
@@ -16667,7 +16740,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>189</v>
       </c>
@@ -16737,8 +16810,11 @@
       <c r="W198" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X198" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="199" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>192</v>
       </c>
@@ -16812,7 +16888,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>22</v>
       </c>
@@ -16886,7 +16962,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>33</v>
       </c>
@@ -16960,7 +17036,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>57</v>
       </c>
@@ -17031,7 +17107,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>42</v>
       </c>
@@ -17102,7 +17178,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>183</v>
       </c>
@@ -17176,7 +17252,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>186</v>
       </c>
@@ -17247,7 +17323,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>189</v>
       </c>
@@ -17317,8 +17393,11 @@
       <c r="W206" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X206" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="207" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>192</v>
       </c>
@@ -17392,7 +17471,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>22</v>
       </c>
@@ -17466,7 +17545,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>33</v>
       </c>
@@ -17540,7 +17619,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>57</v>
       </c>
@@ -17611,7 +17690,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>42</v>
       </c>
@@ -17682,7 +17761,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>22</v>
       </c>
@@ -17756,7 +17835,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>33</v>
       </c>
@@ -17830,7 +17909,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>57</v>
       </c>
@@ -17901,7 +17980,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>42</v>
       </c>
@@ -17972,7 +18051,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>183</v>
       </c>
@@ -18046,7 +18125,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>186</v>
       </c>
@@ -18117,7 +18196,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>189</v>
       </c>
@@ -18187,8 +18266,11 @@
       <c r="W218" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X218" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="219" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>192</v>
       </c>
@@ -18262,7 +18344,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>22</v>
       </c>
@@ -18336,7 +18418,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>33</v>
       </c>
@@ -18410,7 +18492,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>57</v>
       </c>
@@ -18481,7 +18563,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>42</v>
       </c>
@@ -18552,7 +18634,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>183</v>
       </c>
@@ -18626,7 +18708,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>186</v>
       </c>
@@ -18697,7 +18779,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>189</v>
       </c>
@@ -18767,8 +18849,11 @@
       <c r="W226" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X226" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="227" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>192</v>
       </c>
@@ -18842,7 +18927,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>22</v>
       </c>
@@ -18916,7 +19001,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>33</v>
       </c>
@@ -18990,7 +19075,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>57</v>
       </c>
@@ -19061,7 +19146,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>42</v>
       </c>
@@ -19132,7 +19217,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>183</v>
       </c>
@@ -19206,7 +19291,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>186</v>
       </c>
@@ -19277,7 +19362,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>189</v>
       </c>
@@ -19347,8 +19432,11 @@
       <c r="W234" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X234" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="235" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>192</v>
       </c>
@@ -19419,7 +19507,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>22</v>
       </c>
@@ -19493,7 +19581,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>33</v>
       </c>
@@ -19567,7 +19655,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>57</v>
       </c>
@@ -19638,7 +19726,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>42</v>
       </c>
@@ -19709,7 +19797,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>22</v>
       </c>
@@ -19783,7 +19871,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>33</v>
       </c>
@@ -19857,7 +19945,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>57</v>
       </c>
@@ -19928,7 +20016,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>42</v>
       </c>
@@ -19999,7 +20087,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>183</v>
       </c>
@@ -20073,7 +20161,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>186</v>
       </c>
@@ -20144,7 +20232,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>189</v>
       </c>
@@ -20214,8 +20302,11 @@
       <c r="W246" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X246" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="247" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>192</v>
       </c>
@@ -20289,7 +20380,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>22</v>
       </c>
@@ -20363,7 +20454,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>33</v>
       </c>
@@ -20437,7 +20528,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>57</v>
       </c>
@@ -20508,7 +20599,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>42</v>
       </c>
@@ -20579,7 +20670,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>183</v>
       </c>
@@ -20653,7 +20744,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>186</v>
       </c>
@@ -20724,7 +20815,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>189</v>
       </c>
@@ -20794,8 +20885,11 @@
       <c r="W254" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X254" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="255" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>192</v>
       </c>
@@ -20869,7 +20963,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>22</v>
       </c>
@@ -20943,7 +21037,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>33</v>
       </c>
@@ -21017,7 +21111,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>57</v>
       </c>
@@ -21088,7 +21182,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>42</v>
       </c>
@@ -21159,7 +21253,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>183</v>
       </c>
@@ -21233,7 +21327,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>186</v>
       </c>
@@ -21304,7 +21398,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>189</v>
       </c>
@@ -21374,8 +21468,11 @@
       <c r="W262" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X262" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="263" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>192</v>
       </c>
@@ -21449,7 +21546,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>22</v>
       </c>
@@ -21523,7 +21620,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>33</v>
       </c>
@@ -21597,7 +21694,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>57</v>
       </c>
@@ -21668,7 +21765,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>42</v>
       </c>
@@ -21739,7 +21836,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>183</v>
       </c>
@@ -21813,7 +21910,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>186</v>
       </c>
@@ -21884,7 +21981,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>189</v>
       </c>
@@ -21954,8 +22051,11 @@
       <c r="W270" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X270" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="271" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>192</v>
       </c>
@@ -22029,7 +22129,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>22</v>
       </c>
@@ -22103,7 +22203,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>33</v>
       </c>
@@ -22177,7 +22277,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>57</v>
       </c>
@@ -22248,7 +22348,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>42</v>
       </c>
@@ -22319,7 +22419,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>183</v>
       </c>
@@ -22393,7 +22493,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>186</v>
       </c>
@@ -22464,7 +22564,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>189</v>
       </c>
@@ -22534,8 +22634,11 @@
       <c r="W278" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X278" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="279" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>192</v>
       </c>
@@ -22609,7 +22712,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>22</v>
       </c>
@@ -22683,7 +22786,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>33</v>
       </c>
@@ -22757,7 +22860,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>57</v>
       </c>
@@ -22828,7 +22931,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>42</v>
       </c>
@@ -22899,7 +23002,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>183</v>
       </c>
@@ -22973,7 +23076,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>186</v>
       </c>
@@ -23044,7 +23147,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>189</v>
       </c>
@@ -23114,8 +23217,11 @@
       <c r="W286" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X286" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="287" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>192</v>
       </c>
@@ -23189,7 +23295,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>22</v>
       </c>
@@ -23263,7 +23369,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>33</v>
       </c>
@@ -23337,7 +23443,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="290" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>57</v>
       </c>
@@ -23408,7 +23514,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="291" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>22</v>
       </c>
@@ -23482,7 +23588,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="292" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>33</v>
       </c>
@@ -23556,7 +23662,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="293" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>57</v>
       </c>
@@ -23627,7 +23733,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="294" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>42</v>
       </c>
@@ -23698,7 +23804,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="295" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>183</v>
       </c>
@@ -23772,7 +23878,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="296" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>186</v>
       </c>
@@ -23843,7 +23949,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="297" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>189</v>
       </c>
@@ -23913,8 +24019,11 @@
       <c r="W297" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="298" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X297" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="298" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>192</v>
       </c>
@@ -23988,7 +24097,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="299" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>22</v>
       </c>
@@ -24062,7 +24171,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="300" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>33</v>
       </c>
@@ -24136,7 +24245,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="301" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>57</v>
       </c>
@@ -24207,7 +24316,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="302" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>42</v>
       </c>
@@ -24278,7 +24387,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="303" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>183</v>
       </c>
@@ -24352,7 +24461,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="304" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>186</v>
       </c>
@@ -24423,7 +24532,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="305" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>189</v>
       </c>
@@ -24493,8 +24602,11 @@
       <c r="W305" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="306" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X305" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="306" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>192</v>
       </c>
@@ -24568,7 +24680,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="307" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>22</v>
       </c>
@@ -24642,7 +24754,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="308" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>33</v>
       </c>
@@ -24716,7 +24828,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="309" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>57</v>
       </c>
@@ -24787,7 +24899,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="310" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>42</v>
       </c>
@@ -24858,7 +24970,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="311" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>183</v>
       </c>
@@ -24932,7 +25044,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="312" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>186</v>
       </c>
@@ -25003,7 +25115,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="313" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>189</v>
       </c>
@@ -25073,8 +25185,11 @@
       <c r="W313" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="314" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X313" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="314" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>192</v>
       </c>
@@ -25148,7 +25263,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="315" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>22</v>
       </c>
@@ -25222,7 +25337,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="316" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>33</v>
       </c>
@@ -25296,7 +25411,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="317" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>57</v>
       </c>
@@ -25367,7 +25482,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="318" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>42</v>
       </c>
@@ -25438,7 +25553,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="319" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>22</v>
       </c>
@@ -25512,7 +25627,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="320" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>33</v>
       </c>
@@ -25586,7 +25701,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="321" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>57</v>
       </c>
@@ -25657,7 +25772,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="322" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>42</v>
       </c>
@@ -25728,7 +25843,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="323" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>183</v>
       </c>
@@ -25802,7 +25917,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="324" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>186</v>
       </c>
@@ -25873,7 +25988,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="325" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>189</v>
       </c>
@@ -25943,8 +26058,11 @@
       <c r="W325" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="326" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X325" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="326" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>192</v>
       </c>
@@ -26018,7 +26136,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="327" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>22</v>
       </c>
@@ -26092,7 +26210,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="328" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>33</v>
       </c>
@@ -26166,7 +26284,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="329" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>57</v>
       </c>
@@ -26237,7 +26355,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="330" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>42</v>
       </c>
@@ -26308,7 +26426,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="331" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>183</v>
       </c>
@@ -26382,7 +26500,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="332" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>186</v>
       </c>
@@ -26453,7 +26571,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="333" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>189</v>
       </c>
@@ -26523,8 +26641,11 @@
       <c r="W333" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="334" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X333" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="334" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>192</v>
       </c>
@@ -26598,7 +26719,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="335" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>22</v>
       </c>
@@ -26672,7 +26793,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="336" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>33</v>
       </c>
@@ -26746,7 +26867,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="337" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>57</v>
       </c>
@@ -26817,7 +26938,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="338" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>42</v>
       </c>
@@ -26888,7 +27009,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="339" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>183</v>
       </c>
@@ -26962,7 +27083,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="340" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>186</v>
       </c>
@@ -27033,7 +27154,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="341" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>189</v>
       </c>
@@ -27103,8 +27224,11 @@
       <c r="W341" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="342" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X341" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="342" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>192</v>
       </c>
@@ -27178,7 +27302,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="343" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>22</v>
       </c>
@@ -27252,7 +27376,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="344" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>57</v>
       </c>
@@ -27323,7 +27447,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="345" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>42</v>
       </c>
@@ -27394,7 +27518,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="346" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>183</v>
       </c>
@@ -27468,7 +27592,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="347" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>186</v>
       </c>
@@ -27539,7 +27663,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="348" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>189</v>
       </c>
@@ -27609,8 +27733,11 @@
       <c r="W348" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="349" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X348" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="349" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>192</v>
       </c>
@@ -27684,7 +27811,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="350" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>22</v>
       </c>
@@ -27758,7 +27885,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="351" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>33</v>
       </c>
@@ -27832,7 +27959,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="352" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>57</v>
       </c>
@@ -27903,7 +28030,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="353" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>42</v>
       </c>
@@ -27974,7 +28101,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="354" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>183</v>
       </c>
@@ -28048,7 +28175,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="355" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>186</v>
       </c>
@@ -28119,7 +28246,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="356" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>189</v>
       </c>
@@ -28189,8 +28316,11 @@
       <c r="W356" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="357" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X356" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="357" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>192</v>
       </c>
@@ -28264,7 +28394,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="358" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>22</v>
       </c>
@@ -28338,7 +28468,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="359" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>33</v>
       </c>
@@ -28412,7 +28542,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="360" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>57</v>
       </c>
@@ -28483,7 +28613,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="361" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>42</v>
       </c>
@@ -28554,7 +28684,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="362" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>183</v>
       </c>
@@ -28628,7 +28758,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="363" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>186</v>
       </c>
@@ -28699,7 +28829,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="364" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>189</v>
       </c>
@@ -28769,8 +28899,11 @@
       <c r="W364" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="365" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X364" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="365" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>192</v>
       </c>
@@ -28844,7 +28977,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="366" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>22</v>
       </c>
@@ -28918,7 +29051,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="367" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>33</v>
       </c>
@@ -28992,7 +29125,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="368" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>57</v>
       </c>
@@ -29063,7 +29196,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="369" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>42</v>
       </c>
@@ -29134,7 +29267,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="370" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>186</v>
       </c>
@@ -29205,7 +29338,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="371" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>189</v>
       </c>
@@ -29275,8 +29408,11 @@
       <c r="W371" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="372" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X371" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="372" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>192</v>
       </c>
@@ -29350,7 +29486,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="373" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>57</v>
       </c>
@@ -29421,7 +29557,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="374" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>42</v>
       </c>
@@ -29492,7 +29628,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="375" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>183</v>
       </c>
@@ -29566,7 +29702,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="376" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>186</v>
       </c>
@@ -29637,7 +29773,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="377" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>189</v>
       </c>
@@ -29707,8 +29843,11 @@
       <c r="W377" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="378" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X377" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="378" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>192</v>
       </c>
@@ -29782,7 +29921,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="379" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>22</v>
       </c>
@@ -29856,7 +29995,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="380" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>33</v>
       </c>
@@ -29930,7 +30069,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="381" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>57</v>
       </c>
@@ -30001,7 +30140,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="382" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>42</v>
       </c>
@@ -30072,7 +30211,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="383" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>183</v>
       </c>
@@ -30146,7 +30285,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="384" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>186</v>
       </c>
@@ -30217,7 +30356,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="385" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>189</v>
       </c>
@@ -30287,8 +30426,11 @@
       <c r="W385" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="386" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X385" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="386" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>192</v>
       </c>
@@ -30362,7 +30504,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="387" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>22</v>
       </c>
@@ -30436,7 +30578,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="388" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>33</v>
       </c>
@@ -30510,7 +30652,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="389" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>57</v>
       </c>
@@ -30581,7 +30723,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="390" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>42</v>
       </c>
@@ -30652,7 +30794,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="391" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>42</v>
       </c>
@@ -30723,7 +30865,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="392" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>186</v>
       </c>
@@ -30794,7 +30936,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="393" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>189</v>
       </c>
@@ -30864,8 +31006,11 @@
       <c r="W393" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="394" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X393" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="394" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>192</v>
       </c>
@@ -30939,7 +31084,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="395" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>186</v>
       </c>
@@ -31010,7 +31155,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="396" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>189</v>
       </c>
@@ -31080,8 +31225,11 @@
       <c r="W396" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="397" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X396" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="397" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>192</v>
       </c>
@@ -31155,7 +31303,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="398" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>57</v>
       </c>
@@ -31226,7 +31374,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="399" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>42</v>
       </c>
@@ -31297,7 +31445,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="400" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>189</v>
       </c>
@@ -31367,8 +31515,11 @@
       <c r="W400" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="401" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X400" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="401" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>192</v>
       </c>
@@ -31442,7 +31593,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="402" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>22</v>
       </c>
@@ -31516,7 +31667,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="403" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>33</v>
       </c>
@@ -31590,7 +31741,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="404" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>57</v>
       </c>
@@ -31661,7 +31812,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="405" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>42</v>
       </c>
@@ -31732,7 +31883,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="406" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>42</v>
       </c>
@@ -31803,7 +31954,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="407" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>186</v>
       </c>
@@ -31874,7 +32025,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="408" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>189</v>
       </c>
@@ -31944,8 +32095,11 @@
       <c r="W408" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="409" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X408" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="409" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>192</v>
       </c>
@@ -32019,7 +32173,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="410" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>42</v>
       </c>
@@ -32090,7 +32244,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="411" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>186</v>
       </c>
@@ -32161,7 +32315,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="412" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>189</v>
       </c>
@@ -32231,8 +32385,11 @@
       <c r="W412" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="413" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X412" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="413" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>192</v>
       </c>
@@ -32306,7 +32463,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="414" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>189</v>
       </c>
@@ -32376,8 +32533,11 @@
       <c r="W414" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="415" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X414" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="415" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>192</v>
       </c>
@@ -32451,7 +32611,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="416" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>186</v>
       </c>
@@ -32522,7 +32682,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="417" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>186</v>
       </c>
@@ -32593,7 +32753,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="418" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>22</v>
       </c>
@@ -32667,7 +32827,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="419" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>22</v>
       </c>
@@ -32741,7 +32901,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="420" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>33</v>
       </c>
@@ -32815,7 +32975,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="421" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>57</v>
       </c>
@@ -32886,7 +33046,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="422" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>57</v>
       </c>
@@ -32957,7 +33117,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="423" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>22</v>
       </c>
@@ -33031,7 +33191,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="424" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>33</v>
       </c>
@@ -33105,7 +33265,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="425" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>42</v>
       </c>
@@ -33176,7 +33336,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="426" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>22</v>
       </c>
@@ -33250,7 +33410,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="427" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>33</v>
       </c>
@@ -33324,7 +33484,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="428" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>57</v>
       </c>
@@ -33395,7 +33555,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="429" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>22</v>
       </c>
@@ -33469,7 +33629,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="430" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>33</v>
       </c>
@@ -33543,7 +33703,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="431" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>22</v>
       </c>
@@ -33617,7 +33777,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="432" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>42</v>
       </c>
@@ -33688,7 +33848,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="433" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>183</v>
       </c>
@@ -33762,8 +33922,24 @@
         <v>399</v>
       </c>
     </row>
+    <row r="434" spans="1:24" hidden="1" x14ac:dyDescent="0.25">
+      <c r="X434" t="s">
+        <v>499</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:W433" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:W434" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Cow"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="21">
+      <filters>
+        <filter val="Bovine Influenza"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>